<commit_message>
Agregada Columna Telefono del Elector en Reporte SegVoto SIP
</commit_message>
<xml_diff>
--- a/src/Pequiven/SEIPBundle/Resources/Skeleton/Sip/SegVoto.xlsx
+++ b/src/Pequiven/SEIPBundle/Resources/Skeleton/Sip/SegVoto.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="519"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="419"/>
   </bookViews>
   <sheets>
     <sheet name="Cuadro" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cuadro!$A$4:$O$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cuadro!$A$4:$P$4</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">Cuadro!$A$4:$M$5</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="0">Cuadro!$A$4:$M$5</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="0">Cuadro!$A$4:$M$5</definedName>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Sistema de Información Política</t>
   </si>
@@ -96,7 +91,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -246,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -284,15 +279,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -308,9 +294,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -319,6 +302,21 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -384,15 +382,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>530678</xdr:colOff>
+      <xdr:colOff>68035</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>217714</xdr:rowOff>
+      <xdr:rowOff>204107</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>707571</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1020536</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1224643</xdr:rowOff>
+      <xdr:rowOff>1211036</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -405,7 +403,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24764999" y="217714"/>
+          <a:off x="24302356" y="204107"/>
           <a:ext cx="952501" cy="1006929"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -464,7 +462,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -499,7 +497,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -676,7 +674,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -687,10 +685,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
@@ -704,22 +702,24 @@
     <col min="7" max="7" width="20" style="8" customWidth="1"/>
     <col min="8" max="10" width="26.7109375" style="8" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="22" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="18" customWidth="1"/>
     <col min="13" max="13" width="35.7109375" style="8" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="2"/>
-    <col min="15" max="15" width="41" style="2" customWidth="1"/>
-    <col min="16" max="1019" width="11.5703125" style="2"/>
-    <col min="1020" max="16384" width="9.140625" style="2"/>
+    <col min="14" max="14" width="20" style="8" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="2"/>
+    <col min="16" max="16" width="41" style="2" customWidth="1"/>
+    <col min="17" max="1020" width="11.5703125" style="2"/>
+    <col min="1021" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K1" s="11"/>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="11"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="11"/>
     </row>
-    <row r="2" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>11</v>
       </c>
@@ -735,37 +735,39 @@
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
       <c r="M2" s="21"/>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="25"/>
+      <c r="O2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="13" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="13" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="13" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="12"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -806,37 +808,41 @@
         <v>1</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="20"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="17"/>
       <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:O4"/>
+  <autoFilter ref="A4:P4"/>
   <mergeCells count="5">
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="L3:M3"/>
     <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:O3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.39370078740157483" footer="0.39370078740157483"/>

</xml_diff>